<commit_message>
updated project plan for rest of year by quarters
</commit_message>
<xml_diff>
--- a/project-management-template-sjg.xlsx
+++ b/project-management-template-sjg.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\sjg\2021\self\training\udacity\nanodegree\final project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CA50550-198D-4A2B-A23E-04E1A73D66D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC09E90F-36DD-4F8C-8EAF-4E12BBC55E70}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="CICD Pipeline" sheetId="1" r:id="rId1"/>
+    <sheet name="3Q21" sheetId="2" r:id="rId2"/>
+    <sheet name="4Q21" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="62">
   <si>
     <t>Week</t>
   </si>
@@ -124,12 +126,105 @@
   <si>
     <t>Get locust testing working with locustfile.py</t>
   </si>
+  <si>
+    <t>Overall Objectives for 3Q21</t>
+  </si>
+  <si>
+    <t>Overall Objectives for 4Q21</t>
+  </si>
+  <si>
+    <t>Link in a Jupyter notebook for the Boston Housing ML model as another pipeline, deploying the joblib or a pickle file to Github and then doing the application build and deploy.</t>
+  </si>
+  <si>
+    <t>Add testing and collect coverage metrics</t>
+  </si>
+  <si>
+    <t>Build an image and push to Azure Container Registry</t>
+  </si>
+  <si>
+    <t>Set up Kubernetes environment</t>
+  </si>
+  <si>
+    <t>Automate the Kubernetes environment setup with Terraform</t>
+  </si>
+  <si>
+    <t>Deploy the application on Kubernetes</t>
+  </si>
+  <si>
+    <t>Build automation to deploy the application to Kubernetes</t>
+  </si>
+  <si>
+    <t>Introduce auto-scaling to enable Kubernetes to grow the number of instances based on load</t>
+  </si>
+  <si>
+    <t>Document experiments in auto-scaling</t>
+  </si>
+  <si>
+    <t>Update README and code to incorporate Kubernetes setup and deployment</t>
+  </si>
+  <si>
+    <t>Set up wiki to answer additional questions</t>
+  </si>
+  <si>
+    <t>Document test results</t>
+  </si>
+  <si>
+    <t>Test new application and predictions; make bug fixes</t>
+  </si>
+  <si>
+    <t>Add additional functions to the Azure Pipeline</t>
+  </si>
+  <si>
+    <t>Set up Jupyter notebook environment</t>
+  </si>
+  <si>
+    <t>Build initial notebook for the model</t>
+  </si>
+  <si>
+    <t>Experiment with different models</t>
+  </si>
+  <si>
+    <t>Evaluate models based on accuracy, recall, precision, F1 score, and ROC curve</t>
+  </si>
+  <si>
+    <t>Save the best model using joblib or pickle</t>
+  </si>
+  <si>
+    <t>Insert model in a flask application</t>
+  </si>
+  <si>
+    <t>Build a container for the application and model</t>
+  </si>
+  <si>
+    <t>Deploy the containerized application</t>
+  </si>
+  <si>
+    <t>Set up an A/B test for the new application vs. existing application</t>
+  </si>
+  <si>
+    <t>Document results of the experiment</t>
+  </si>
+  <si>
+    <t>If new application predicts better than the existing application, replace existing</t>
+  </si>
+  <si>
+    <t>Document model approach and results</t>
+  </si>
+  <si>
+    <t>Update readme to include creation, testing, and deployment of a new model</t>
+  </si>
+  <si>
+    <t>Deploy new readme</t>
+  </si>
+  <si>
+    <t>Drive and test auto-scaling through locust; see number of instances test; need LB in front</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -162,6 +257,25 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF24292E"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -189,7 +303,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -204,6 +318,9 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -424,8 +541,8 @@
   </sheetPr>
   <dimension ref="A1:Z1014"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29:D29"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -29072,4 +29189,396 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7F141E9-FA8C-4D6A-8670-6CBFD82FEC83}">
+  <dimension ref="A1:C17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="74.88671875" customWidth="1"/>
+    <col min="3" max="3" width="27.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>44375</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
+        <v>44382</v>
+      </c>
+      <c r="B3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="5">
+        <v>44389</v>
+      </c>
+      <c r="B4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="5">
+        <v>44396</v>
+      </c>
+      <c r="B5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="5">
+        <v>44403</v>
+      </c>
+      <c r="B6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="5">
+        <v>44410</v>
+      </c>
+      <c r="B7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="5">
+        <v>44417</v>
+      </c>
+      <c r="B8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="5">
+        <v>44424</v>
+      </c>
+      <c r="B9" t="s">
+        <v>61</v>
+      </c>
+      <c r="C9" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="5">
+        <v>44431</v>
+      </c>
+      <c r="B10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="5">
+        <v>44438</v>
+      </c>
+      <c r="B11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="5">
+        <v>44445</v>
+      </c>
+      <c r="B12" t="s">
+        <v>43</v>
+      </c>
+      <c r="C12" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="5">
+        <v>44452</v>
+      </c>
+      <c r="B13" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="5">
+        <v>44459</v>
+      </c>
+      <c r="B14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C15">
+        <f>SUM(C2:C14)</f>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B16" s="12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>46</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B60CA397-3BA4-4376-B959-3BCAA9C14E76}">
+  <dimension ref="A1:C18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.21875" customWidth="1"/>
+    <col min="2" max="2" width="80.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>44466</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
+        <v>44473</v>
+      </c>
+      <c r="B3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="5">
+        <v>44480</v>
+      </c>
+      <c r="B4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="5">
+        <v>44487</v>
+      </c>
+      <c r="B5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="5">
+        <v>44494</v>
+      </c>
+      <c r="B6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="5">
+        <v>44501</v>
+      </c>
+      <c r="B7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="5">
+        <v>44508</v>
+      </c>
+      <c r="B8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="5">
+        <v>44515</v>
+      </c>
+      <c r="B9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="5">
+        <v>44522</v>
+      </c>
+      <c r="B10" t="s">
+        <v>55</v>
+      </c>
+      <c r="C10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="5">
+        <v>44529</v>
+      </c>
+      <c r="B11" t="s">
+        <v>56</v>
+      </c>
+      <c r="C11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="5">
+        <v>44536</v>
+      </c>
+      <c r="B12" t="s">
+        <v>57</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="5">
+        <v>44543</v>
+      </c>
+      <c r="B13" t="s">
+        <v>58</v>
+      </c>
+      <c r="C13">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="5">
+        <v>44550</v>
+      </c>
+      <c r="B14" t="s">
+        <v>59</v>
+      </c>
+      <c r="C14">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="5">
+        <v>44557</v>
+      </c>
+      <c r="B15" t="s">
+        <v>60</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C16">
+        <f>SUM(C2:C15)</f>
+        <v>78</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" s="12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" ht="15" x14ac:dyDescent="0.35">
+      <c r="B18" s="13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>